<commit_message>
Commit before deleting some extra old files
</commit_message>
<xml_diff>
--- a/Cocktails.xlsx
+++ b/Cocktails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a47020f47dca8947/Documents/Cocktails/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhsch\Documents\Development\CocktailRecipes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="8_{232A2F8D-D117-4F44-847F-2A22E59A3DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E79192F8-C469-4F33-8389-16576BC50E44}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3430E195-AA48-48EF-9E44-B6A401ED3558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{B7EC54BE-E733-418F-92A4-376D983B0AE8}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{B7EC54BE-E733-418F-92A4-376D983B0AE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipe" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
   <si>
     <t>Number</t>
   </si>
@@ -229,9 +229,6 @@
     <t>ABV</t>
   </si>
   <si>
-    <t>Whisky</t>
-  </si>
-  <si>
     <t>Water - Dilution</t>
   </si>
   <si>
@@ -263,16 +260,65 @@
   </si>
   <si>
     <t>Grenadine</t>
+  </si>
+  <si>
+    <t>ml_mg</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w_v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>spirit</t>
+  </si>
+  <si>
+    <t>bitters</t>
+  </si>
+  <si>
+    <t>liquor</t>
+  </si>
+  <si>
+    <t>syrup</t>
+  </si>
+  <si>
+    <t>dairy</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>fortified wine</t>
+  </si>
+  <si>
+    <t>ref gm per ml</t>
+  </si>
+  <si>
+    <t>ref ABV</t>
+  </si>
+  <si>
+    <t>https://bartenderly.com/tips-tricks/alcohol-density-chart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +341,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -304,7 +358,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -312,13 +366,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -328,8 +392,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
@@ -347,14 +416,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -392,7 +457,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -498,7 +563,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -640,7 +705,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -654,9 +719,9 @@
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
@@ -682,7 +747,7 @@
       </c>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -747,7 +812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -800,7 +865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -856,7 +921,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -930,55 +995,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC84C39-09BD-44C2-A2CF-DDB940D61B5F}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2">
         <v>29.574000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3">
         <v>4.9289199999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4">
         <v>14.786799999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
       <c r="B5">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -986,13 +1066,41 @@
         <f>B5</f>
         <v>0.92</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7">
         <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1002,33 +1110,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D34C318-C563-4D62-ADF0-11B0E5DFE4EC}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="3"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="3"/>
+    <col min="4" max="4" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="8"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1038,11 +1158,22 @@
       <c r="C2" s="3">
         <v>40</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="8">
+        <f>IF(ISBLANK(B2),VLOOKUP(D2,A:E,5,),B2)</f>
+        <v>0.93520000000000003</v>
+      </c>
+      <c r="F2" s="8">
+        <f>IF(ISBLANK(C2),VLOOKUP(D2,A:F,6,),C2)</f>
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1052,11 +1183,22 @@
       <c r="C3" s="3">
         <v>44.7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E20" si="0">IF(ISBLANK(B3),VLOOKUP(D3,A:E,5,),B3)</f>
+        <v>0.93</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F20" si="1">IF(ISBLANK(C3),VLOOKUP(D3,A:F,6,),C3)</f>
+        <v>44.7</v>
+      </c>
+      <c r="G3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1066,8 +1208,19 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
+        <v>1.22</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1078,8 +1231,19 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>1.2650000000000001</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1089,80 +1253,273 @@
       <c r="C6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>1.31</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
       <c r="B7">
-        <v>0.93520000000000003</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>1.034</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>64</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="8" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F9" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.97</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="8" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="8" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>0.93520000000000003</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="8" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="D16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="0"/>
+        <v>0.97</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <v>1.18</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" si="0"/>
+        <v>1.18</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>84</v>
+      </c>
+      <c r="B18">
+        <v>1.034</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" si="0"/>
+        <v>1.034</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19">
+        <v>0.94</v>
+      </c>
+      <c r="C19" s="3">
+        <v>40</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20">
+        <v>0.97</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" si="0"/>
+        <v>0.97</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="1"/>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>